<commit_message>
Did effect of number of trees in the forest
</commit_message>
<xml_diff>
--- a/Intermediate Results.xlsx
+++ b/Intermediate Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\link4\Documents\CodeStuff\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA3CE77-3A54-4B34-A77F-0BC732FC1C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5A4B8-95B3-41C0-BB9B-78C1C7CDA925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
   <si>
     <t>Type</t>
   </si>
@@ -237,6 +237,15 @@
       </rPr>
       <t>, 0.000010015, 'Learner', 'leastsquares', 'Regularization', 'ridge', 'Solver', 'bfgs' (columns: model, year, mileage, fuel type, MPG, engine size), Normalised</t>
     </r>
+  </si>
+  <si>
+    <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 450, (columns: model, year, mileage, fuel type, MPG, engine size).</t>
+  </si>
+  <si>
+    <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 50, (columns: model, year, mileage, fuel type, MPG, engine size).</t>
+  </si>
+  <si>
+    <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 500, (columns: model, year, mileage, fuel type, MPG, engine size).</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -440,6 +449,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,11 +998,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFAFB13-90C1-41EC-B846-648BA9BFAA48}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,6 +1198,57 @@
         <v>0.94</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1175.03</v>
+      </c>
+      <c r="D12" s="16">
+        <v>838.63</v>
+      </c>
+      <c r="E12" s="16">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1178.42</v>
+      </c>
+      <c r="D13" s="16">
+        <v>839.35</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1174.68</v>
+      </c>
+      <c r="D14" s="16">
+        <v>838.28</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ran KFold on linear regression
Need to do the same for Random Forest
</commit_message>
<xml_diff>
--- a/Intermediate Results.xlsx
+++ b/Intermediate Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\link4\Documents\CodeStuff\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E5A4B8-95B3-41C0-BB9B-78C1C7CDA925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0184CF-49F4-4731-8176-E5A96CDF983C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
+    <workbookView xWindow="22725" yWindow="3225" windowWidth="12105" windowHeight="12150" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Type</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 500, (columns: model, year, mileage, fuel type, MPG, engine size).</t>
+  </si>
+  <si>
+    <t>Lambda', 0.000010015, 'Learner', 'leastsquares', 'Regularization', 'ridge', 'Solver', 'bfgs', 'Kfold', 5 (columns: model, year, mileage, fuel type, MPG, engine size), Normalised (1st model)</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -453,6 +456,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFAFB13-90C1-41EC-B846-648BA9BFAA48}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,104 +1120,104 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="16">
         <v>1826.26</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="16">
         <v>1347.21</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="16">
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1818.02</v>
+      </c>
+      <c r="D8" s="14">
+        <v>1344.83</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C9" s="11">
         <v>1279.6600000000001</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D9" s="11">
         <v>889.33</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E9" s="11">
         <v>0.93</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C10" s="11">
         <v>1185.69</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D10" s="11">
         <v>837.56</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E10" s="11">
         <v>0.94</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C11" s="11">
         <v>1398.75</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D11" s="11">
         <v>968.24</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E11" s="11">
         <v>0.91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C12" s="14">
         <v>1175.02</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D12" s="14">
         <v>838.02</v>
       </c>
-      <c r="E11" s="14">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1175.03</v>
-      </c>
-      <c r="D12" s="16">
-        <v>838.63</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="E12" s="14">
         <v>0.94</v>
       </c>
     </row>
@@ -1220,13 +1226,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="16">
-        <v>1178.42</v>
+        <v>1175.03</v>
       </c>
       <c r="D13" s="16">
-        <v>839.35</v>
+        <v>838.63</v>
       </c>
       <c r="E13" s="16">
         <v>0.94</v>
@@ -1237,15 +1243,32 @@
         <v>8</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1178.42</v>
+      </c>
+      <c r="D14" s="16">
+        <v>839.35</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C15" s="16">
         <v>1174.68</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D15" s="16">
         <v>838.28</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E15" s="16">
         <v>0.94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sorted out Kfold predictions
</commit_message>
<xml_diff>
--- a/Intermediate Results.xlsx
+++ b/Intermediate Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\link4\Documents\CodeStuff\ML-FordUsedCars\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364CB56F-C806-4D8F-A4ED-B9CB72829259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E276EEA1-F678-4166-8C38-D903A264F1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22725" yWindow="3225" windowWidth="12105" windowHeight="12150" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
+    <workbookView xWindow="1260" yWindow="1140" windowWidth="13980" windowHeight="11385" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Results" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Type</t>
   </si>
@@ -252,6 +252,15 @@
   </si>
   <si>
     <t>Due to being given new random numbers</t>
+  </si>
+  <si>
+    <t>Lambda', 0.000010015, 'Learner', 'leastsquares', 'Regularization', 'ridge', 'Solver', 'bfgs', 'Kfold', 5 (columns: model, year, mileage, fuel type, MPG, engine size), Normalised (average of models)</t>
+  </si>
+  <si>
+    <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 499, (columns: model, year, mileage, fuel type, MPG, engine size). Kfold (average of models)</t>
+  </si>
+  <si>
+    <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 50, Kfold, 5, CrossVal, On, (columns: model, year, mileage, fuel type, MPG, engine size). Kfold (average of models)</t>
   </si>
 </sst>
 </file>
@@ -314,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -411,11 +420,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,6 +482,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -957,7 +982,7 @@
         <v>892.84</v>
       </c>
     </row>
-    <row r="13" spans="1:4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1007,11 +1032,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFAFB13-90C1-41EC-B846-648BA9BFAA48}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1045,7 @@
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1037,7 +1062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1079,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -1071,7 +1096,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
@@ -1088,7 +1113,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -1105,7 +1130,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
@@ -1122,7 +1147,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
@@ -1139,7 +1164,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1156,143 +1181,194 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:5" s="18" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1826.27</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1347.26</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C10" s="11">
         <v>1279.6600000000001</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D10" s="11">
         <v>889.33</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E10" s="11">
         <v>0.93</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C11" s="11">
         <v>1185.69</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D11" s="11">
         <v>837.56</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E11" s="11">
         <v>0.94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C12" s="11">
         <v>1398.75</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D12" s="11">
         <v>968.24</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E12" s="11">
         <v>0.91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1175.02</v>
-      </c>
-      <c r="D12" s="16">
-        <v>838.02</v>
-      </c>
-      <c r="E12" s="16">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C13" s="16">
-        <v>1175.03</v>
+        <v>1175.02</v>
       </c>
       <c r="D13" s="16">
-        <v>838.63</v>
+        <v>838.02</v>
       </c>
       <c r="E13" s="16">
         <v>0.94</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="16">
-        <v>1178.42</v>
+        <v>1175.03</v>
       </c>
       <c r="D14" s="16">
-        <v>839.35</v>
+        <v>838.63</v>
       </c>
       <c r="E14" s="16">
         <v>0.94</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="16">
-        <v>1174.68</v>
+        <v>1178.42</v>
       </c>
       <c r="D15" s="16">
-        <v>838.28</v>
+        <v>839.35</v>
       </c>
       <c r="E15" s="16">
         <v>0.94</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1174.68</v>
+      </c>
+      <c r="D16" s="16">
+        <v>838.28</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C17" s="14">
         <v>1177.4000000000001</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D17" s="14">
         <v>839.2</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E17" s="14">
         <v>0.94</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="20">
+        <v>1182.52</v>
+      </c>
+      <c r="D18" s="20">
+        <v>843.05</v>
+      </c>
+      <c r="E18" s="20">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="20">
+        <v>1185.95</v>
+      </c>
+      <c r="D19" s="20">
+        <v>842.7</v>
+      </c>
+      <c r="E19" s="20">
+        <v>0.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Random Forest so that it used less trees
</commit_message>
<xml_diff>
--- a/Intermediate Results.xlsx
+++ b/Intermediate Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E276EEA1-F678-4166-8C38-D903A264F1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7987B0B4-5692-455E-A231-9A0E2F587B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1140" windowWidth="13980" windowHeight="11385" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>Type</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 50, Kfold, 5, CrossVal, On, (columns: model, year, mileage, fuel type, MPG, engine size). Kfold (average of models)</t>
+  </si>
+  <si>
+    <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 100, (columns: model, year, mileage, fuel type, MPG, engine size).</t>
   </si>
 </sst>
 </file>
@@ -1032,11 +1035,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFAFB13-90C1-41EC-B846-648BA9BFAA48}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,19 +1321,19 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="A17" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="16">
         <v>1177.4000000000001</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="16">
         <v>839.2</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="16">
         <v>0.94</v>
       </c>
       <c r="F17" t="s">
@@ -1368,6 +1371,23 @@
         <v>842.7</v>
       </c>
       <c r="E19" s="20">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1172.3900000000001</v>
+      </c>
+      <c r="D20" s="14">
+        <v>836.57</v>
+      </c>
+      <c r="E20" s="14">
         <v>0.94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated numbers in the poster for using the new number of trees
</commit_message>
<xml_diff>
--- a/Intermediate Results.xlsx
+++ b/Intermediate Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7987B0B4-5692-455E-A231-9A0E2F587B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A4CFA8-44A2-4A32-AC92-43601EACFD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1140" windowWidth="13980" windowHeight="11385" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Original Results" sheetId="1" r:id="rId1"/>
     <sheet name="New Results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>Type</t>
   </si>
@@ -264,6 +266,9 @@
   </si>
   <si>
     <t>MinLeafSize, 1, Method, Bag, NumLearningCycles, 100, (columns: model, year, mileage, fuel type, MPG, engine size).</t>
+  </si>
+  <si>
+    <t>Hyperparameters</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1043,8 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Excel panicing about phantom changes
</commit_message>
<xml_diff>
--- a/Intermediate Results.xlsx
+++ b/Intermediate Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\ML-FordUsedCars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A4CFA8-44A2-4A32-AC92-43601EACFD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADBF3CA-E1DD-4D97-AECC-14B9B562CBC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1140" windowWidth="13980" windowHeight="11385" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
+    <workbookView xWindow="12435" yWindow="2310" windowWidth="13980" windowHeight="11385" activeTab="1" xr2:uid="{E249E2B7-D0FC-4994-9216-EF814AFAE3A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Results" sheetId="1" r:id="rId1"/>
@@ -1043,8 +1043,8 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>